<commit_message>
Changes to case1_home data input
Ma non ancora risolto optimization
Demand calore ancora da rivedere su distribuzione oraria
</commit_message>
<xml_diff>
--- a/thesis/case1_home/Concettuale_caso1_casa.xlsx
+++ b/thesis/case1_home/Concettuale_caso1_casa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cami/Documents/GitHub/pyesm_tesi/thesis/case1_home/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400268E7-0BE9-6440-ABD6-1E75F715D30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B770B65F-6D49-A54C-9365-EFC40E28EF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{7B02621E-B7BE-C640-8F0D-21B2A43A72CA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{7B02621E-B7BE-C640-8F0D-21B2A43A72CA}"/>
   </bookViews>
   <sheets>
     <sheet name="casa_mia" sheetId="19" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="0" hidden="1">0</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="0" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">casa_mia!$AZ$10:$BF$17,casa_mia!$S$49:$AI$55,casa_mia!$BP$19,casa_mia!$CA$10:$CG$17,casa_mia!$AK$81:$AX$81</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">casa_mia!$AZ$10:$BF$17,casa_mia!$S$49:$AI$55,casa_mia!$BP$19,casa_mia!$CA$10:$CG$17,casa_mia!$AK$83:$AX$83</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
@@ -39,7 +39,7 @@
     <definedName name="solver_lhs18" localSheetId="0" hidden="1">casa_mia!$CA$58:$CG$59</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">casa_mia!$W$49:$X$55</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">casa_mia!$Z$49:$AI$55</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">casa_mia!$AK$81:$AX$81</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">casa_mia!$AK$83:$AX$83</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">casa_mia!$BP$19</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">casa_mia!$BS$10:$BY$17</definedName>
     <definedName name="solver_lhs7" localSheetId="0" hidden="1">casa_mia!$BS$19:$BY$26</definedName>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="200">
   <si>
     <t>time_day</t>
   </si>
@@ -787,6 +787,21 @@
   <si>
     <t>d*X'-Q = 0</t>
   </si>
+  <si>
+    <t>capacity units</t>
+  </si>
+  <si>
+    <t>new_units</t>
+  </si>
+  <si>
+    <t>discount rate</t>
+  </si>
+  <si>
+    <t>1/(1+r)^y</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
 </sst>
 </file>
 
@@ -1103,7 +1118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1169,6 +1184,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1533,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4863A36B-7B9D-4D44-8E2F-FF44385CC5F2}">
-  <dimension ref="A1:CH86"/>
+  <dimension ref="A1:CH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="AL15" sqref="AL15"/>
+    <sheetView tabSelected="1" topLeftCell="P25" zoomScale="75" workbookViewId="0">
+      <selection activeCell="AA44" sqref="AA44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1556,6 +1576,7 @@
     <col min="18" max="18" width="5.6640625" customWidth="1"/>
     <col min="31" max="32" width="14.6640625" customWidth="1"/>
     <col min="36" max="36" width="6.33203125" customWidth="1"/>
+    <col min="43" max="43" width="16" customWidth="1"/>
     <col min="51" max="51" width="4.83203125" customWidth="1"/>
     <col min="59" max="59" width="4.5" customWidth="1"/>
     <col min="61" max="61" width="15.5" customWidth="1"/>
@@ -2312,7 +2333,7 @@
         <v>26</v>
       </c>
       <c r="AQ8" s="9" t="s">
-        <v>26</v>
+        <v>193</v>
       </c>
       <c r="AR8" s="9" t="s">
         <v>26</v>
@@ -2450,7 +2471,7 @@
         <v>0</v>
       </c>
       <c r="V10" s="62">
-        <v>1.0000000000000001E-5</v>
+        <v>0.05</v>
       </c>
       <c r="W10" s="62">
         <f>1/3.6</f>
@@ -2563,13 +2584,13 @@
       <c r="BR10" s="13"/>
       <c r="BS10" s="17" cm="1">
         <f t="array" ref="BS10:BY17">AZ10:BF17-MMULT(S10:AI17,TRANSPOSE(S49:AI55))-BH10:BN17*_xlfn.ANCHORARRAY(BQ10)-CA10:CG17</f>
-        <v>-5.3249999666604708E-5</v>
+        <v>-0.26666658166666757</v>
       </c>
       <c r="BT10" s="18">
         <v>2.2222224060897133E-8</v>
       </c>
       <c r="BU10" s="18">
-        <v>-1.833333366718648E-5</v>
+        <v>-9.3333001666666249E-2</v>
       </c>
       <c r="BV10" s="18">
         <v>0</v>
@@ -2627,12 +2648,12 @@
         <v>2386.6341527700001</v>
       </c>
       <c r="K11" s="31" cm="1">
-        <f t="array" ref="K11">MMULT(AK38:AX38,TRANSPOSE(AK81:AX81))+BP19*BP21</f>
-        <v>1340</v>
+        <f t="array" ref="K11">MMULT(AK38:AX38,TRANSPOSE(AK83:AX83))+BP19*BP21</f>
+        <v>640</v>
       </c>
       <c r="L11" s="32">
-        <f>J11+K11</f>
-        <v>3726.6341527700001</v>
+        <f>J11*SUM(J81:J90)+K11</f>
+        <v>20571.616420323739</v>
       </c>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -2655,7 +2676,7 @@
       <c r="X11" s="14">
         <v>0</v>
       </c>
-      <c r="Y11" s="62">
+      <c r="Y11" s="15">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="Z11" s="15">
@@ -2814,7 +2835,9 @@
         <v>26</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="J12" s="3" t="s">
+        <v>197</v>
+      </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -3000,7 +3023,9 @@
         <v>26</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="J13" s="66">
+        <v>4.2500000000000003E-2</v>
+      </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -3183,7 +3208,7 @@
         <v>40</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>26</v>
+        <v>193</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -4328,25 +4353,25 @@
       </c>
       <c r="BZ20" s="13"/>
       <c r="CA20" s="20">
-        <v>3.4706104</v>
+        <v>1.7706103999999989</v>
       </c>
       <c r="CB20" s="13">
-        <v>4.9222222000000002</v>
+        <v>3.2222221999999991</v>
       </c>
       <c r="CC20" s="13">
-        <v>0</v>
+        <v>-1.7000000000000011</v>
       </c>
       <c r="CD20" s="13">
-        <v>0.5</v>
+        <v>-1.2000000000000011</v>
       </c>
       <c r="CE20" s="13">
-        <v>6.9</v>
+        <v>5.1999999999999993</v>
       </c>
       <c r="CF20" s="21">
-        <v>0.30000000000000071</v>
+        <v>-1.4000000000000004</v>
       </c>
       <c r="CG20">
-        <v>0</v>
+        <v>-1.7000000000000011</v>
       </c>
     </row>
     <row r="21" spans="1:85" x14ac:dyDescent="0.2">
@@ -4962,25 +4987,25 @@
       </c>
       <c r="BZ24" s="13"/>
       <c r="CA24" s="20">
-        <v>1.5</v>
+        <v>5.5</v>
       </c>
       <c r="CB24" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="CC24" s="13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="CD24" s="13">
-        <v>1.5</v>
+        <v>5.5</v>
       </c>
       <c r="CE24" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="CF24" s="21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="CG24">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:85" x14ac:dyDescent="0.2">
@@ -5113,25 +5138,25 @@
       </c>
       <c r="BZ25" s="13"/>
       <c r="CA25" s="20">
-        <v>9998.8857821599995</v>
+        <v>57.885782159999998</v>
       </c>
       <c r="CB25" s="13">
-        <v>9998.7715643299998</v>
+        <v>57.771564329999997</v>
       </c>
       <c r="CC25" s="13">
-        <v>9998.5431286500007</v>
+        <v>57.54312865</v>
       </c>
       <c r="CD25" s="13">
-        <v>9998.8857821599995</v>
+        <v>57.885782159999998</v>
       </c>
       <c r="CE25" s="13">
-        <v>9998.7715643299998</v>
+        <v>57.771564329999997</v>
       </c>
       <c r="CF25" s="21">
-        <v>9998.5431286500007</v>
+        <v>57.54312865</v>
       </c>
       <c r="CG25">
-        <v>9998.5431286500007</v>
+        <v>57.54312865</v>
       </c>
     </row>
     <row r="26" spans="1:85" x14ac:dyDescent="0.2">
@@ -5178,7 +5203,7 @@
       <c r="Y26" s="13"/>
       <c r="Z26" s="13"/>
       <c r="AA26" s="13"/>
-      <c r="AB26" s="13"/>
+      <c r="AB26" s="63"/>
       <c r="AC26" s="13"/>
       <c r="AD26" s="13"/>
       <c r="AE26" s="13"/>
@@ -5564,7 +5589,7 @@
         <v>19</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>26</v>
+        <v>193</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="14">
@@ -6424,7 +6449,7 @@
       <c r="BR35" s="13"/>
       <c r="BZ35" s="13"/>
       <c r="CA35" s="13" cm="1">
-        <f t="array" ref="CA35:CC35">AT81:AV81</f>
+        <f t="array" ref="CA35:CC35">AT83:AV83</f>
         <v>0</v>
       </c>
       <c r="CB35" s="13">
@@ -6477,7 +6502,7 @@
         <v>0.1</v>
       </c>
       <c r="U37" s="14">
-        <v>-0.05</v>
+        <v>-0.08</v>
       </c>
       <c r="V37" s="14">
         <v>0</v>
@@ -6587,25 +6612,25 @@
         <v>57</v>
       </c>
       <c r="AK38" s="16">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="AL38" s="16">
         <v>100</v>
       </c>
       <c r="AM38" s="16">
-        <v>2000</v>
-      </c>
-      <c r="AN38" s="16">
+        <v>3000</v>
+      </c>
+      <c r="AN38" s="60">
         <v>500</v>
       </c>
       <c r="AO38" s="16">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="AP38" s="16">
-        <v>500</v>
+        <v>150</v>
       </c>
       <c r="AQ38" s="16">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="AR38" s="16">
         <v>1000</v>
@@ -6698,8 +6723,8 @@
       <c r="AP39" s="16">
         <v>0</v>
       </c>
-      <c r="AQ39" s="61">
-        <v>9999</v>
+      <c r="AQ39" s="16">
+        <v>58</v>
       </c>
       <c r="AR39" s="16">
         <v>3.5</v>
@@ -8911,42 +8936,42 @@
         <v>0</v>
       </c>
       <c r="AK57" s="33" cm="1">
-        <f t="array" ref="AK57:AL62">AK49:AL54*$AW$83:$AX$83</f>
+        <f t="array" ref="AK57:AL62">AK49:AL54*$AW$87:$AX$87</f>
         <v>1.8</v>
       </c>
       <c r="AL57" s="33">
         <v>0</v>
       </c>
       <c r="AM57" s="33" cm="1">
-        <f t="array" ref="AM57:AN62">AM49:AN54*$AW$83:$AX$83</f>
+        <f t="array" ref="AM57:AN62">AM49:AN54*$AW$87:$AX$87</f>
         <v>16.2</v>
       </c>
       <c r="AN57" s="33">
         <v>6.8970000000000002</v>
       </c>
       <c r="AO57" s="33" cm="1">
-        <f t="array" ref="AO57:AP62">AO49:AP54*$AW$83:$AX$83</f>
+        <f t="array" ref="AO57:AP62">AO49:AP54*$AW$87:$AX$87</f>
         <v>9</v>
       </c>
       <c r="AP57" s="33">
         <v>3.4833333333333334</v>
       </c>
       <c r="AQ57" s="33" cm="1">
-        <f t="array" ref="AQ57:AR63">AQ49:AR55*$AW$83:$AX$83</f>
+        <f t="array" ref="AQ57:AR63">AQ49:AR55*$AW$87:$AX$87</f>
         <v>10.799999999999999</v>
       </c>
       <c r="AR57" s="33">
         <v>5.5733333333333341</v>
       </c>
       <c r="AS57" s="33" cm="1">
-        <f t="array" ref="AS57:AT63">AS49:AT55*$AW$83:$AX$83</f>
+        <f t="array" ref="AS57:AT63">AS49:AT55*$AW$87:$AX$87</f>
         <v>-10.799999999999999</v>
       </c>
       <c r="AT57" s="33">
         <v>-5.5733333333333341</v>
       </c>
       <c r="AZ57" s="33" cm="1">
-        <f t="array" ref="AZ57:BB62">AZ49:BB54*AU83</f>
+        <f t="array" ref="AZ57:BB62">AZ49:BB54*AU87</f>
         <v>5</v>
       </c>
       <c r="BA57" s="33">
@@ -9671,11 +9696,11 @@
         <v>0</v>
       </c>
       <c r="AK65" s="33" cm="1">
-        <f t="array" ref="AK65:AV71">MMULT(AK41:AV47,_xlfn.MUNIT(12)*AK83:AV83)</f>
+        <f t="array" ref="AK65:AV71">MMULT(AK41:AV47,_xlfn.MUNIT(12)*AK87:AV87)</f>
         <v>0.9</v>
       </c>
       <c r="AL65" s="34">
-        <v>12.4</v>
+        <v>10.7</v>
       </c>
       <c r="AM65" s="34">
         <v>6</v>
@@ -9687,10 +9712,10 @@
         <v>0</v>
       </c>
       <c r="AP65" s="34">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AQ65" s="34">
-        <v>9999</v>
+        <v>58</v>
       </c>
       <c r="AR65" s="34">
         <v>3.5</v>
@@ -9743,7 +9768,7 @@
         <v>1.8</v>
       </c>
       <c r="AL66" s="34">
-        <v>12.4</v>
+        <v>10.7</v>
       </c>
       <c r="AM66" s="34">
         <v>6</v>
@@ -9755,10 +9780,10 @@
         <v>0</v>
       </c>
       <c r="AP66" s="34">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AQ66" s="34">
-        <v>9999</v>
+        <v>58</v>
       </c>
       <c r="AR66" s="34">
         <v>0</v>
@@ -9817,7 +9842,7 @@
         <v>0.9</v>
       </c>
       <c r="AL67" s="34">
-        <v>12.4</v>
+        <v>10.7</v>
       </c>
       <c r="AM67" s="34">
         <v>6</v>
@@ -9829,10 +9854,10 @@
         <v>0</v>
       </c>
       <c r="AP67" s="34">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AQ67" s="34">
-        <v>9999</v>
+        <v>58</v>
       </c>
       <c r="AR67" s="34">
         <v>3.5</v>
@@ -9892,7 +9917,7 @@
         <v>1.8</v>
       </c>
       <c r="AL68" s="34">
-        <v>12.4</v>
+        <v>10.7</v>
       </c>
       <c r="AM68" s="34">
         <v>6</v>
@@ -9904,10 +9929,10 @@
         <v>0</v>
       </c>
       <c r="AP68" s="34">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AQ68" s="34">
-        <v>9999</v>
+        <v>58</v>
       </c>
       <c r="AR68" s="34">
         <v>3.5</v>
@@ -9966,7 +9991,7 @@
         <v>2.6999999999999997</v>
       </c>
       <c r="AL69" s="34">
-        <v>12.4</v>
+        <v>10.7</v>
       </c>
       <c r="AM69" s="34">
         <v>6</v>
@@ -9978,10 +10003,10 @@
         <v>0</v>
       </c>
       <c r="AP69" s="34">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AQ69" s="34">
-        <v>9999</v>
+        <v>58</v>
       </c>
       <c r="AR69" s="34">
         <v>0</v>
@@ -10046,7 +10071,7 @@
         <v>1.8</v>
       </c>
       <c r="AL70" s="34">
-        <v>12.4</v>
+        <v>10.7</v>
       </c>
       <c r="AM70" s="34">
         <v>6</v>
@@ -10058,10 +10083,10 @@
         <v>0</v>
       </c>
       <c r="AP70" s="34">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AQ70" s="34">
-        <v>9999</v>
+        <v>58</v>
       </c>
       <c r="AR70" s="34">
         <v>3.5</v>
@@ -10126,7 +10151,7 @@
         <v>0</v>
       </c>
       <c r="AL71" s="34">
-        <v>12.4</v>
+        <v>10.7</v>
       </c>
       <c r="AM71" s="34">
         <v>6</v>
@@ -10138,10 +10163,10 @@
         <v>0</v>
       </c>
       <c r="AP71" s="34">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AQ71" s="34">
-        <v>9999</v>
+        <v>58</v>
       </c>
       <c r="AR71" s="34">
         <v>0</v>
@@ -10229,7 +10254,7 @@
       <c r="Q73" s="3"/>
       <c r="R73" s="3"/>
       <c r="W73" s="59" cm="1">
-        <f t="array" ref="W73:X79">W65:X71*W83:X83</f>
+        <f t="array" ref="W73:X79">W65:X71*W87:X87</f>
         <v>6</v>
       </c>
       <c r="X73" s="34">
@@ -10744,13 +10769,20 @@
       </c>
     </row>
     <row r="80" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
-      <c r="H80" s="10"/>
+      <c r="H80" s="10" t="s">
+        <v>199</v>
+      </c>
       <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
+      <c r="J80" s="3" t="s">
+        <v>198</v>
+      </c>
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
       <c r="M80" s="3"/>
@@ -10759,9 +10791,22 @@
       <c r="P80" s="3"/>
       <c r="Q80" s="3"/>
       <c r="R80" s="3"/>
-      <c r="AK80" s="11" t="s">
-        <v>90</v>
-      </c>
+      <c r="AK80" s="64" t="s">
+        <v>195</v>
+      </c>
+      <c r="AL80" s="64"/>
+      <c r="AM80" s="64"/>
+      <c r="AN80" s="64"/>
+      <c r="AO80" s="64"/>
+      <c r="AP80" s="64"/>
+      <c r="AQ80" s="64"/>
+      <c r="AR80" s="64"/>
+      <c r="AS80" s="64"/>
+      <c r="AT80" s="64"/>
+      <c r="AU80" s="64"/>
+      <c r="AV80" s="64"/>
+      <c r="AW80" s="64"/>
+      <c r="AX80" s="64"/>
     </row>
     <row r="81" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
@@ -10771,9 +10816,14 @@
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
-      <c r="H81" s="10"/>
+      <c r="H81" s="67">
+        <v>0</v>
+      </c>
       <c r="I81" s="3"/>
-      <c r="J81" s="3"/>
+      <c r="J81" s="3">
+        <f>1/(1+$J$13)^H81</f>
+        <v>1</v>
+      </c>
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
       <c r="M81" s="3"/>
@@ -10782,47 +10832,47 @@
       <c r="P81" s="3"/>
       <c r="Q81" s="3"/>
       <c r="R81" s="3"/>
-      <c r="AK81" s="22">
-        <v>0</v>
-      </c>
-      <c r="AL81" s="22">
-        <v>3.4</v>
-      </c>
-      <c r="AM81" s="22">
-        <v>0</v>
-      </c>
-      <c r="AN81" s="22">
-        <v>0</v>
-      </c>
-      <c r="AO81" s="22">
-        <v>0</v>
-      </c>
-      <c r="AP81" s="22">
-        <v>2</v>
-      </c>
-      <c r="AQ81" s="22">
-        <v>0</v>
-      </c>
-      <c r="AR81" s="22">
-        <v>0</v>
-      </c>
-      <c r="AS81" s="22">
-        <v>0</v>
-      </c>
-      <c r="AT81" s="22">
-        <v>0</v>
-      </c>
-      <c r="AU81" s="22">
-        <v>0</v>
-      </c>
-      <c r="AV81" s="22">
-        <v>0</v>
-      </c>
-      <c r="AW81" s="22">
-        <v>0</v>
-      </c>
-      <c r="AX81" s="22">
-        <v>0</v>
+      <c r="AK81" s="65">
+        <v>1</v>
+      </c>
+      <c r="AL81" s="65">
+        <v>0.5</v>
+      </c>
+      <c r="AM81" s="65">
+        <v>5</v>
+      </c>
+      <c r="AN81" s="65">
+        <v>1</v>
+      </c>
+      <c r="AO81" s="65">
+        <v>3</v>
+      </c>
+      <c r="AP81" s="65">
+        <v>3</v>
+      </c>
+      <c r="AQ81" s="65">
+        <v>0</v>
+      </c>
+      <c r="AR81" s="65">
+        <v>7</v>
+      </c>
+      <c r="AS81" s="65">
+        <v>0</v>
+      </c>
+      <c r="AT81" s="65">
+        <v>0</v>
+      </c>
+      <c r="AU81" s="65">
+        <v>0</v>
+      </c>
+      <c r="AV81" s="65">
+        <v>160</v>
+      </c>
+      <c r="AW81" s="65">
+        <v>3</v>
+      </c>
+      <c r="AX81" s="65">
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:50" x14ac:dyDescent="0.2">
@@ -10833,9 +10883,14 @@
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
-      <c r="H82" s="10"/>
+      <c r="H82" s="67">
+        <v>1</v>
+      </c>
       <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
+      <c r="J82" s="3">
+        <f>1/(1+$J$13)^H82</f>
+        <v>0.95923261390887293</v>
+      </c>
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
       <c r="M82" s="3"/>
@@ -10844,11 +10899,8 @@
       <c r="P82" s="3"/>
       <c r="Q82" s="3"/>
       <c r="R82" s="3"/>
-      <c r="S82" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="AK82" s="11" t="s">
-        <v>70</v>
+      <c r="AK82" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="83" spans="1:50" x14ac:dyDescent="0.2">
@@ -10859,9 +10911,14 @@
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
-      <c r="H83" s="10"/>
+      <c r="H83" s="67">
+        <v>2</v>
+      </c>
       <c r="I83" s="3"/>
-      <c r="J83" s="3"/>
+      <c r="J83" s="3">
+        <f t="shared" ref="J83:J90" si="0">1/(1+$J$13)^H83</f>
+        <v>0.92012720758644884</v>
+      </c>
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
       <c r="M83" s="3"/>
@@ -10870,113 +10927,62 @@
       <c r="P83" s="3"/>
       <c r="Q83" s="3"/>
       <c r="R83" s="3"/>
-      <c r="S83" s="34" cm="1">
-        <f t="array" ref="S83:AI83">MMULT(_xlfn.ANCHORARRAY(AK83),TRANSPOSE(AK19:AX35))</f>
-        <v>9</v>
-      </c>
-      <c r="T83" s="34">
-        <v>12.4</v>
-      </c>
-      <c r="U83" s="34">
-        <v>12.4</v>
-      </c>
-      <c r="V83" s="34">
-        <v>18</v>
-      </c>
-      <c r="W83" s="34">
-        <v>6</v>
-      </c>
-      <c r="X83" s="34">
-        <v>6</v>
-      </c>
-      <c r="Y83" s="34">
-        <v>6.9666666666666668</v>
-      </c>
-      <c r="Z83" s="34">
-        <v>100</v>
-      </c>
-      <c r="AA83" s="34">
-        <v>0</v>
-      </c>
-      <c r="AB83" s="34">
+      <c r="AK83" s="22">
+        <v>0</v>
+      </c>
+      <c r="AL83" s="22">
+        <v>3.4</v>
+      </c>
+      <c r="AM83" s="22">
+        <v>0</v>
+      </c>
+      <c r="AN83" s="22">
+        <v>0</v>
+      </c>
+      <c r="AO83" s="22">
+        <v>0</v>
+      </c>
+      <c r="AP83" s="22">
         <v>2</v>
       </c>
-      <c r="AC83" s="34">
-        <v>9999</v>
-      </c>
-      <c r="AD83" s="34">
-        <v>3.5</v>
-      </c>
-      <c r="AE83" s="34">
-        <v>82</v>
-      </c>
-      <c r="AF83" s="34">
-        <v>82</v>
-      </c>
-      <c r="AG83" s="34">
-        <v>100</v>
-      </c>
-      <c r="AH83" s="34">
-        <v>160</v>
-      </c>
-      <c r="AI83" s="34">
-        <v>160</v>
-      </c>
-      <c r="AK83" s="35" cm="1">
-        <f t="array" ref="AK83:AX83">(AK81:AX81+AK39:AX39)</f>
-        <v>9</v>
-      </c>
-      <c r="AL83" s="35">
-        <v>12.4</v>
-      </c>
-      <c r="AM83" s="35">
-        <v>6</v>
-      </c>
-      <c r="AN83" s="35">
-        <v>100</v>
-      </c>
-      <c r="AO83" s="35">
-        <v>0</v>
-      </c>
-      <c r="AP83" s="35">
-        <v>2</v>
-      </c>
-      <c r="AQ83" s="41">
-        <v>9999</v>
-      </c>
-      <c r="AR83" s="35">
-        <v>3.5</v>
-      </c>
-      <c r="AS83" s="35">
-        <v>22</v>
-      </c>
-      <c r="AT83" s="35">
-        <v>60</v>
-      </c>
-      <c r="AU83" s="35">
-        <v>100</v>
-      </c>
-      <c r="AV83" s="35">
-        <v>160</v>
-      </c>
-      <c r="AW83" s="35">
-        <v>18</v>
-      </c>
-      <c r="AX83" s="35">
-        <v>6.9666666666666668</v>
+      <c r="AQ83" s="22">
+        <v>0</v>
+      </c>
+      <c r="AR83" s="22">
+        <v>0</v>
+      </c>
+      <c r="AS83" s="22">
+        <v>0</v>
+      </c>
+      <c r="AT83" s="22">
+        <v>0</v>
+      </c>
+      <c r="AU83" s="22">
+        <v>0</v>
+      </c>
+      <c r="AV83" s="22">
+        <v>0</v>
+      </c>
+      <c r="AW83" s="22">
+        <v>0</v>
+      </c>
+      <c r="AX83" s="22">
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
-      <c r="H84" s="10"/>
+      <c r="H84" s="67">
+        <v>3</v>
+      </c>
       <c r="I84" s="3"/>
-      <c r="J84" s="3"/>
+      <c r="J84" s="3">
+        <f t="shared" si="0"/>
+        <v>0.88261602646182147</v>
+      </c>
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
       <c r="M84" s="3"/>
@@ -10985,6 +10991,9 @@
       <c r="P84" s="3"/>
       <c r="Q84" s="3"/>
       <c r="R84" s="3"/>
+      <c r="AK84" s="11" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="85" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A85" s="3"/>
@@ -10994,9 +11003,14 @@
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
-      <c r="H85" s="10"/>
+      <c r="H85" s="67">
+        <v>4</v>
+      </c>
       <c r="I85" s="3"/>
-      <c r="J85" s="3"/>
+      <c r="J85" s="3">
+        <f t="shared" si="0"/>
+        <v>0.84663407814083602</v>
+      </c>
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
       <c r="M85" s="3"/>
@@ -11005,6 +11019,49 @@
       <c r="P85" s="3"/>
       <c r="Q85" s="3"/>
       <c r="R85" s="3"/>
+      <c r="AK85" s="34" cm="1">
+        <f t="array" ref="AK85:AX85">AK83:AX83*AK81:AX81</f>
+        <v>0</v>
+      </c>
+      <c r="AL85" s="34">
+        <v>1.7</v>
+      </c>
+      <c r="AM85" s="34">
+        <v>0</v>
+      </c>
+      <c r="AN85" s="34">
+        <v>0</v>
+      </c>
+      <c r="AO85" s="34">
+        <v>0</v>
+      </c>
+      <c r="AP85" s="34">
+        <v>6</v>
+      </c>
+      <c r="AQ85" s="34">
+        <v>0</v>
+      </c>
+      <c r="AR85" s="34">
+        <v>0</v>
+      </c>
+      <c r="AS85" s="34">
+        <v>0</v>
+      </c>
+      <c r="AT85" s="34">
+        <v>0</v>
+      </c>
+      <c r="AU85" s="34">
+        <v>0</v>
+      </c>
+      <c r="AV85" s="34">
+        <v>0</v>
+      </c>
+      <c r="AW85" s="34">
+        <v>0</v>
+      </c>
+      <c r="AX85" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="86" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A86" s="3"/>
@@ -11014,9 +11071,14 @@
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
-      <c r="H86" s="10"/>
+      <c r="H86" s="67">
+        <v>5</v>
+      </c>
       <c r="I86" s="3"/>
-      <c r="J86" s="3"/>
+      <c r="J86" s="3">
+        <f t="shared" si="0"/>
+        <v>0.81211901979936307</v>
+      </c>
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
       <c r="M86" s="3"/>
@@ -11025,6 +11087,207 @@
       <c r="P86" s="3"/>
       <c r="Q86" s="3"/>
       <c r="R86" s="3"/>
+      <c r="S86" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK86" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="87" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="67">
+        <v>6</v>
+      </c>
+      <c r="I87" s="3"/>
+      <c r="J87" s="3">
+        <f t="shared" si="0"/>
+        <v>0.7790110501672548</v>
+      </c>
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+      <c r="M87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="3"/>
+      <c r="P87" s="3"/>
+      <c r="Q87" s="3"/>
+      <c r="R87" s="3"/>
+      <c r="S87" s="34" cm="1">
+        <f t="array" ref="S87:AI87">MMULT(_xlfn.ANCHORARRAY(AK87),TRANSPOSE(AK19:AX35))</f>
+        <v>9</v>
+      </c>
+      <c r="T87" s="34">
+        <v>10.7</v>
+      </c>
+      <c r="U87" s="34">
+        <v>10.7</v>
+      </c>
+      <c r="V87" s="34">
+        <v>18</v>
+      </c>
+      <c r="W87" s="34">
+        <v>6</v>
+      </c>
+      <c r="X87" s="34">
+        <v>6</v>
+      </c>
+      <c r="Y87" s="34">
+        <v>6.9666666666666668</v>
+      </c>
+      <c r="Z87" s="34">
+        <v>100</v>
+      </c>
+      <c r="AA87" s="34">
+        <v>0</v>
+      </c>
+      <c r="AB87" s="34">
+        <v>6</v>
+      </c>
+      <c r="AC87" s="34">
+        <v>58</v>
+      </c>
+      <c r="AD87" s="34">
+        <v>3.5</v>
+      </c>
+      <c r="AE87" s="34">
+        <v>82</v>
+      </c>
+      <c r="AF87" s="34">
+        <v>82</v>
+      </c>
+      <c r="AG87" s="34">
+        <v>100</v>
+      </c>
+      <c r="AH87" s="34">
+        <v>160</v>
+      </c>
+      <c r="AI87" s="34">
+        <v>160</v>
+      </c>
+      <c r="AK87" s="35" cm="1">
+        <f t="array" ref="AK87:AX87">(_xlfn.ANCHORARRAY(AK85)+AK39:AX39)</f>
+        <v>9</v>
+      </c>
+      <c r="AL87" s="35">
+        <v>10.7</v>
+      </c>
+      <c r="AM87" s="35">
+        <v>6</v>
+      </c>
+      <c r="AN87" s="35">
+        <v>100</v>
+      </c>
+      <c r="AO87" s="35">
+        <v>0</v>
+      </c>
+      <c r="AP87" s="35">
+        <v>6</v>
+      </c>
+      <c r="AQ87" s="41">
+        <v>58</v>
+      </c>
+      <c r="AR87" s="35">
+        <v>3.5</v>
+      </c>
+      <c r="AS87" s="35">
+        <v>22</v>
+      </c>
+      <c r="AT87" s="35">
+        <v>60</v>
+      </c>
+      <c r="AU87" s="35">
+        <v>100</v>
+      </c>
+      <c r="AV87" s="35">
+        <v>160</v>
+      </c>
+      <c r="AW87" s="35">
+        <v>18</v>
+      </c>
+      <c r="AX87" s="35">
+        <v>6.9666666666666668</v>
+      </c>
+    </row>
+    <row r="88" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="67">
+        <v>7</v>
+      </c>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3">
+        <f t="shared" si="0"/>
+        <v>0.74725280591583187</v>
+      </c>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="3"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="3"/>
+      <c r="P88" s="3"/>
+      <c r="Q88" s="3"/>
+      <c r="R88" s="3"/>
+    </row>
+    <row r="89" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="67">
+        <v>8</v>
+      </c>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3">
+        <f t="shared" si="0"/>
+        <v>0.71678926226938311</v>
+      </c>
+      <c r="K89" s="3"/>
+      <c r="L89" s="3"/>
+      <c r="M89" s="3"/>
+      <c r="N89" s="3"/>
+      <c r="O89" s="3"/>
+      <c r="P89" s="3"/>
+      <c r="Q89" s="3"/>
+      <c r="R89" s="3"/>
+    </row>
+    <row r="90" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="67">
+        <v>9</v>
+      </c>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3">
+        <f t="shared" si="0"/>
+        <v>0.68756763766847306</v>
+      </c>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+      <c r="P90" s="3"/>
+      <c r="Q90" s="3"/>
+      <c r="R90" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>

</xml_diff>

<commit_message>
cambi nomi e grafici
</commit_message>
<xml_diff>
--- a/thesis/case1_home/Concettuale_caso1_casa.xlsx
+++ b/thesis/case1_home/Concettuale_caso1_casa.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cami/Documents/GitHub/pyesm_tesi/thesis/case1_home/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B770B65F-6D49-A54C-9365-EFC40E28EF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FBF71E-7F0B-BE4D-A2D9-CBB59255C40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{7B02621E-B7BE-C640-8F0D-21B2A43A72CA}"/>
   </bookViews>
   <sheets>
-    <sheet name="casa_mia" sheetId="19" r:id="rId1"/>
+    <sheet name="home_buccinasco" sheetId="19" r:id="rId1"/>
     <sheet name="time_accurate" sheetId="21" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -21,35 +21,35 @@
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="0" hidden="1">0</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="0" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">casa_mia!$AZ$10:$BF$17,casa_mia!$S$49:$AI$55,casa_mia!$BP$19,casa_mia!$CA$10:$CG$17,casa_mia!$AK$83:$AX$83</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">home_buccinasco!$AZ$10:$BF$17,home_buccinasco!$S$49:$AI$55,home_buccinasco!$BP$19,home_buccinasco!$CA$10:$CG$17,home_buccinasco!$AK$83:$AX$83</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">casa_mia!$S$49:$U$55</definedName>
-    <definedName name="solver_lhs10" localSheetId="0" hidden="1">casa_mia!$CA$35:$CC$35</definedName>
-    <definedName name="solver_lhs11" localSheetId="0" hidden="1">casa_mia!$CA$37:$CG$39</definedName>
-    <definedName name="solver_lhs12" localSheetId="0" hidden="1">casa_mia!$CA$41:$CF$42</definedName>
-    <definedName name="solver_lhs13" localSheetId="0" hidden="1">casa_mia!$CA$44:$CF$45</definedName>
-    <definedName name="solver_lhs14" localSheetId="0" hidden="1">casa_mia!$CA$47:$CG$48</definedName>
-    <definedName name="solver_lhs15" localSheetId="0" hidden="1">casa_mia!$CA$50:$CG$51</definedName>
-    <definedName name="solver_lhs16" localSheetId="0" hidden="1">casa_mia!$CA$53:$CF$53</definedName>
-    <definedName name="solver_lhs17" localSheetId="0" hidden="1">casa_mia!$CA$55:$CF$55</definedName>
-    <definedName name="solver_lhs18" localSheetId="0" hidden="1">casa_mia!$CA$58:$CG$59</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">casa_mia!$W$49:$X$55</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">casa_mia!$Z$49:$AI$55</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">casa_mia!$AK$83:$AX$83</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">casa_mia!$BP$19</definedName>
-    <definedName name="solver_lhs6" localSheetId="0" hidden="1">casa_mia!$BS$10:$BY$17</definedName>
-    <definedName name="solver_lhs7" localSheetId="0" hidden="1">casa_mia!$BS$19:$BY$26</definedName>
-    <definedName name="solver_lhs8" localSheetId="0" hidden="1">casa_mia!$CA$10:$CG$17</definedName>
-    <definedName name="solver_lhs9" localSheetId="0" hidden="1">casa_mia!$CA$19:$CG$30</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">home_buccinasco!$S$49:$U$55</definedName>
+    <definedName name="solver_lhs10" localSheetId="0" hidden="1">home_buccinasco!$CA$35:$CC$35</definedName>
+    <definedName name="solver_lhs11" localSheetId="0" hidden="1">home_buccinasco!$CA$37:$CG$39</definedName>
+    <definedName name="solver_lhs12" localSheetId="0" hidden="1">home_buccinasco!$CA$41:$CF$42</definedName>
+    <definedName name="solver_lhs13" localSheetId="0" hidden="1">home_buccinasco!$CA$44:$CF$45</definedName>
+    <definedName name="solver_lhs14" localSheetId="0" hidden="1">home_buccinasco!$CA$47:$CG$48</definedName>
+    <definedName name="solver_lhs15" localSheetId="0" hidden="1">home_buccinasco!$CA$50:$CG$51</definedName>
+    <definedName name="solver_lhs16" localSheetId="0" hidden="1">home_buccinasco!$CA$53:$CF$53</definedName>
+    <definedName name="solver_lhs17" localSheetId="0" hidden="1">home_buccinasco!$CA$55:$CF$55</definedName>
+    <definedName name="solver_lhs18" localSheetId="0" hidden="1">home_buccinasco!$CA$58:$CG$59</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">home_buccinasco!$W$49:$X$55</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">home_buccinasco!$Z$49:$AI$55</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">home_buccinasco!$AK$83:$AX$83</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">home_buccinasco!$BP$19</definedName>
+    <definedName name="solver_lhs6" localSheetId="0" hidden="1">home_buccinasco!$BS$10:$BY$17</definedName>
+    <definedName name="solver_lhs7" localSheetId="0" hidden="1">home_buccinasco!$BS$19:$BY$26</definedName>
+    <definedName name="solver_lhs8" localSheetId="0" hidden="1">home_buccinasco!$CA$10:$CG$17</definedName>
+    <definedName name="solver_lhs9" localSheetId="0" hidden="1">home_buccinasco!$CA$19:$CG$30</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">18</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">casa_mia!$L$11</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">home_buccinasco!$L$11</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel10" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel11" localSheetId="0" hidden="1">3</definedName>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1118,7 +1118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1185,8 +1185,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -1555,8 +1553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4863A36B-7B9D-4D44-8E2F-FF44385CC5F2}">
   <dimension ref="A1:CH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P25" zoomScale="75" workbookViewId="0">
-      <selection activeCell="AA44" sqref="AA44"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3023,7 +3021,7 @@
         <v>26</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="66">
+      <c r="J13" s="64">
         <v>4.2500000000000003E-2</v>
       </c>
       <c r="K13" s="3"/>
@@ -10791,22 +10789,9 @@
       <c r="P80" s="3"/>
       <c r="Q80" s="3"/>
       <c r="R80" s="3"/>
-      <c r="AK80" s="64" t="s">
+      <c r="AK80" t="s">
         <v>195</v>
       </c>
-      <c r="AL80" s="64"/>
-      <c r="AM80" s="64"/>
-      <c r="AN80" s="64"/>
-      <c r="AO80" s="64"/>
-      <c r="AP80" s="64"/>
-      <c r="AQ80" s="64"/>
-      <c r="AR80" s="64"/>
-      <c r="AS80" s="64"/>
-      <c r="AT80" s="64"/>
-      <c r="AU80" s="64"/>
-      <c r="AV80" s="64"/>
-      <c r="AW80" s="64"/>
-      <c r="AX80" s="64"/>
     </row>
     <row r="81" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
@@ -10816,7 +10801,7 @@
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
-      <c r="H81" s="67">
+      <c r="H81" s="65">
         <v>0</v>
       </c>
       <c r="I81" s="3"/>
@@ -10832,46 +10817,46 @@
       <c r="P81" s="3"/>
       <c r="Q81" s="3"/>
       <c r="R81" s="3"/>
-      <c r="AK81" s="65">
-        <v>1</v>
-      </c>
-      <c r="AL81" s="65">
+      <c r="AK81" s="16">
+        <v>1</v>
+      </c>
+      <c r="AL81" s="16">
         <v>0.5</v>
       </c>
-      <c r="AM81" s="65">
+      <c r="AM81" s="16">
         <v>5</v>
       </c>
-      <c r="AN81" s="65">
-        <v>1</v>
-      </c>
-      <c r="AO81" s="65">
+      <c r="AN81" s="16">
+        <v>1</v>
+      </c>
+      <c r="AO81" s="16">
         <v>3</v>
       </c>
-      <c r="AP81" s="65">
+      <c r="AP81" s="16">
         <v>3</v>
       </c>
-      <c r="AQ81" s="65">
-        <v>0</v>
-      </c>
-      <c r="AR81" s="65">
+      <c r="AQ81" s="16">
+        <v>0</v>
+      </c>
+      <c r="AR81" s="16">
         <v>7</v>
       </c>
-      <c r="AS81" s="65">
-        <v>0</v>
-      </c>
-      <c r="AT81" s="65">
-        <v>0</v>
-      </c>
-      <c r="AU81" s="65">
-        <v>0</v>
-      </c>
-      <c r="AV81" s="65">
+      <c r="AS81" s="16">
+        <v>0</v>
+      </c>
+      <c r="AT81" s="16">
+        <v>0</v>
+      </c>
+      <c r="AU81" s="16">
+        <v>0</v>
+      </c>
+      <c r="AV81" s="16">
         <v>160</v>
       </c>
-      <c r="AW81" s="65">
+      <c r="AW81" s="16">
         <v>3</v>
       </c>
-      <c r="AX81" s="65">
+      <c r="AX81" s="16">
         <v>5</v>
       </c>
     </row>
@@ -10883,7 +10868,7 @@
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
-      <c r="H82" s="67">
+      <c r="H82" s="65">
         <v>1</v>
       </c>
       <c r="I82" s="3"/>
@@ -10911,7 +10896,7 @@
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
-      <c r="H83" s="67">
+      <c r="H83" s="65">
         <v>2</v>
       </c>
       <c r="I83" s="3"/>
@@ -10975,7 +10960,7 @@
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
-      <c r="H84" s="67">
+      <c r="H84" s="65">
         <v>3</v>
       </c>
       <c r="I84" s="3"/>
@@ -11003,7 +10988,7 @@
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
-      <c r="H85" s="67">
+      <c r="H85" s="65">
         <v>4</v>
       </c>
       <c r="I85" s="3"/>
@@ -11071,7 +11056,7 @@
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
-      <c r="H86" s="67">
+      <c r="H86" s="65">
         <v>5</v>
       </c>
       <c r="I86" s="3"/>
@@ -11102,7 +11087,7 @@
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
-      <c r="H87" s="67">
+      <c r="H87" s="65">
         <v>6</v>
       </c>
       <c r="I87" s="3"/>
@@ -11222,7 +11207,7 @@
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
-      <c r="H88" s="67">
+      <c r="H88" s="65">
         <v>7</v>
       </c>
       <c r="I88" s="3"/>
@@ -11247,7 +11232,7 @@
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
-      <c r="H89" s="67">
+      <c r="H89" s="65">
         <v>8</v>
       </c>
       <c r="I89" s="3"/>
@@ -11272,7 +11257,7 @@
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
-      <c r="H90" s="67">
+      <c r="H90" s="65">
         <v>9</v>
       </c>
       <c r="I90" s="3"/>

</xml_diff>